<commit_message>
add new feature with 'expense anaysis'
</commit_message>
<xml_diff>
--- a/November.xlsx
+++ b/November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_project\py-db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FFD806-C8C8-49B1-8AEC-3D58C27FF7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296EEAAF-744B-4F1B-ABEC-C35AA531FC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="25820" windowHeight="15620" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="156">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -625,6 +625,30 @@
   </si>
   <si>
     <t>双拼（12）+水（2）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻辣烫（13）+烤肠（5）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>午饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两份六两大米</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2589,8 +2613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5B7EDF-6532-4014-9E3B-D49D9FBA2851}">
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5198,15 +5222,65 @@
       <c r="A123" s="1">
         <v>122</v>
       </c>
+      <c r="B123" s="8">
+        <v>45615</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D123" s="1">
+        <v>-18</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F123" s="1">
+        <f>F122+D123</f>
+        <v>413.45000000000027</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
+      <c r="B124" s="8">
+        <v>45615</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="4">
+        <f>SUM(D122:D123)</f>
+        <v>-32</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F124" s="4">
+        <v>413.45000000000027</v>
+      </c>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>124</v>
+      </c>
+      <c r="B125" s="8">
+        <v>45616</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D125" s="1">
+        <v>-3.2</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F125" s="1">
+        <f>F124+D125</f>
+        <v>410.25000000000028</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: some unclear expression and data update 11.27
</commit_message>
<xml_diff>
--- a/November.xlsx
+++ b/November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_project\py-db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC46CF9-9DAB-414D-BB30-DAAB8E2EECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB99A83E-8A3A-4489-8BF6-94EBE63BCE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="25820" windowHeight="15620" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="214">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -809,6 +809,78 @@
   </si>
   <si>
     <t>包含打车从净月回学校（41.21）+11.15去酒店（120）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>午晚饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记不太清好像是土豆炸鸡套餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入账</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亲爱的勾c发米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洗澡用水卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早午饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇妙小蛋挞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十块钱八个，必须尝尝嘛味</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这就是不想出门的下场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无糖小饮料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中奖瓶盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9点真是尴尬点，啥都没有，既不承上也不启下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平帐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使得数据库与实际账面一致</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2773,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5B7EDF-6532-4014-9E3B-D49D9FBA2851}">
   <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F153" sqref="F153"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5567,7 +5639,7 @@
         <v>162</v>
       </c>
       <c r="F131" s="1">
-        <f>F130+D131</f>
+        <f t="shared" ref="F131:F139" si="6">F130+D131</f>
         <v>357.25000000000028</v>
       </c>
     </row>
@@ -5588,7 +5660,7 @@
         <v>164</v>
       </c>
       <c r="F132" s="1">
-        <f>F131+D132</f>
+        <f t="shared" si="6"/>
         <v>351.25000000000028</v>
       </c>
     </row>
@@ -5609,7 +5681,7 @@
         <v>166</v>
       </c>
       <c r="F133" s="1">
-        <f>F132+D133</f>
+        <f t="shared" si="6"/>
         <v>349.25000000000028</v>
       </c>
     </row>
@@ -5630,7 +5702,7 @@
         <v>168</v>
       </c>
       <c r="F134" s="1">
-        <f>F133+D134</f>
+        <f t="shared" si="6"/>
         <v>347.25000000000028</v>
       </c>
     </row>
@@ -5651,7 +5723,7 @@
         <v>170</v>
       </c>
       <c r="F135" s="1">
-        <f>F134+D135</f>
+        <f t="shared" si="6"/>
         <v>325.25000000000028</v>
       </c>
     </row>
@@ -5672,7 +5744,7 @@
         <v>171</v>
       </c>
       <c r="F136" s="1">
-        <f>F135+D136</f>
+        <f t="shared" si="6"/>
         <v>425.25000000000028</v>
       </c>
       <c r="G136" s="1">
@@ -5699,7 +5771,7 @@
         <v>173</v>
       </c>
       <c r="F137" s="1">
-        <f>F136+D137</f>
+        <f t="shared" si="6"/>
         <v>325.25000000000028</v>
       </c>
     </row>
@@ -5720,7 +5792,7 @@
         <v>175</v>
       </c>
       <c r="F138" s="1">
-        <f>F137+D138</f>
+        <f t="shared" si="6"/>
         <v>319.25000000000028</v>
       </c>
     </row>
@@ -5741,7 +5813,7 @@
         <v>177</v>
       </c>
       <c r="F139" s="1">
-        <f>F138+D139</f>
+        <f t="shared" si="6"/>
         <v>303.25000000000028</v>
       </c>
     </row>
@@ -6049,83 +6121,272 @@
       <c r="A154" s="1">
         <v>153</v>
       </c>
+      <c r="B154" s="8">
+        <v>45621</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D154" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F154" s="1">
+        <f>F153+D154</f>
+        <v>433.63000000000034</v>
+      </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>154</v>
       </c>
+      <c r="B155" s="8">
+        <v>45621</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D155" s="1">
+        <v>10</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F155" s="1">
+        <f>F154+D155</f>
+        <v>443.63000000000034</v>
+      </c>
+      <c r="G155" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H155" s="1">
+        <v>2100</v>
+      </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>155</v>
       </c>
+      <c r="B156" s="8">
+        <v>45621</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D156" s="4">
+        <f>SUM(D150:D155)</f>
+        <v>-181.82999999999998</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F156" s="4">
+        <v>443.63000000000034</v>
+      </c>
+      <c r="G156" s="4"/>
+      <c r="H156" s="4"/>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>156</v>
       </c>
+      <c r="B157" s="8">
+        <v>45622</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D157" s="1">
+        <v>-10</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F157" s="1">
+        <f>F156+D157</f>
+        <v>433.63000000000034</v>
+      </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>157</v>
       </c>
+      <c r="B158" s="8">
+        <v>45622</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D158" s="1">
+        <v>-12</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F158" s="1">
+        <f>F157+D158</f>
+        <v>421.63000000000034</v>
+      </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>158</v>
       </c>
+      <c r="B159" s="8">
+        <v>45622</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D159" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F159" s="1">
+        <f>F158+D159</f>
+        <v>416.63000000000034</v>
+      </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B160" s="8">
+        <v>45622</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D160" s="6">
+        <v>-21.78</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F160" s="1">
+        <f>F159+D160</f>
+        <v>394.85000000000036</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B161" s="8">
+        <v>45622</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D161" s="4">
+        <f>SUM(D157:D160)</f>
+        <v>-48.78</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F161" s="4">
+        <v>394.85000000000036</v>
+      </c>
+      <c r="G161" s="4"/>
+      <c r="H161" s="4"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B162" s="8">
+        <v>45623</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F162" s="1">
+        <f>F161+D162</f>
+        <v>393.85000000000036</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B163" s="8">
+        <v>45623</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D163" s="1">
+        <v>-7.5</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F163" s="1">
+        <f>F162+D163</f>
+        <v>386.35000000000036</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B164" s="8">
+        <v>45623</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D164" s="1">
+        <v>-5.35</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F164" s="1">
+        <f>F163+D164</f>
+        <v>381.00000000000034</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B165" s="8">
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
data update 12.4 for my birthday carnival
</commit_message>
<xml_diff>
--- a/November.xlsx
+++ b/November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_project\py-db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06931863-D67D-497F-8A07-B33C5CDED2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A31C9E1-2CE6-4F7B-916F-426584C4D4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="25820" windowHeight="15620" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="291">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1093,6 +1093,102 @@
   </si>
   <si>
     <t>经典套餐（5.4+2）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信用卡结清</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.8电竞酒店（177）+零食（11）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日小蛋糕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海格给哈利同款</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>啤水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸭货</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸭头，鸭脚，鸡脚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炸货</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蘑菇和鸡柳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北环城路到长春北</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长春北到北环城路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轻轨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北环城路到大学城路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早中饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红烧土豆经典套餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张亮经典套餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饼蛋（7.1）+豆浆（2）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3055,10 +3151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5B7EDF-6532-4014-9E3B-D49D9FBA2851}">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181:A211"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H195" sqref="H195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6869,7 +6965,7 @@
         <v>238</v>
       </c>
       <c r="F178" s="1">
-        <f>F177+D178</f>
+        <f t="shared" ref="F178:F188" si="8">F177+D178</f>
         <v>257.4200000000003</v>
       </c>
     </row>
@@ -6890,7 +6986,7 @@
         <v>241</v>
       </c>
       <c r="F179" s="1">
-        <f>F178+D179</f>
+        <f t="shared" si="8"/>
         <v>78.4200000000003</v>
       </c>
     </row>
@@ -6911,7 +7007,7 @@
         <v>243</v>
       </c>
       <c r="F180" s="1">
-        <f>F179+D180</f>
+        <f t="shared" si="8"/>
         <v>76.620000000000303</v>
       </c>
     </row>
@@ -6932,7 +7028,7 @@
         <v>245</v>
       </c>
       <c r="F181" s="1">
-        <f>F180+D181</f>
+        <f t="shared" si="8"/>
         <v>62.630000000000301</v>
       </c>
     </row>
@@ -6953,7 +7049,7 @@
         <v>247</v>
       </c>
       <c r="F182" s="1">
-        <f>F181+D182</f>
+        <f t="shared" si="8"/>
         <v>58.630000000000301</v>
       </c>
     </row>
@@ -6974,7 +7070,7 @@
         <v>249</v>
       </c>
       <c r="F183" s="1">
-        <f>F182+D183</f>
+        <f t="shared" si="8"/>
         <v>54.630000000000301</v>
       </c>
     </row>
@@ -6995,7 +7091,7 @@
         <v>251</v>
       </c>
       <c r="F184" s="1">
-        <f>F183+D184</f>
+        <f t="shared" si="8"/>
         <v>33.340000000000302</v>
       </c>
     </row>
@@ -7016,7 +7112,7 @@
         <v>238</v>
       </c>
       <c r="F185" s="1">
-        <f>F184+D185</f>
+        <f t="shared" si="8"/>
         <v>34.440000000000303</v>
       </c>
     </row>
@@ -7037,7 +7133,7 @@
         <v>238</v>
       </c>
       <c r="F186" s="1">
-        <f>F185+D186</f>
+        <f t="shared" si="8"/>
         <v>124.44000000000031</v>
       </c>
     </row>
@@ -7058,7 +7154,7 @@
         <v>17843123061</v>
       </c>
       <c r="F187" s="1">
-        <f>F186+D187</f>
+        <f t="shared" si="8"/>
         <v>89.510000000000304</v>
       </c>
     </row>
@@ -7079,7 +7175,7 @@
         <v>13551882222</v>
       </c>
       <c r="F188" s="1">
-        <f>F187+D188</f>
+        <f t="shared" si="8"/>
         <v>17.650000000000304</v>
       </c>
     </row>
@@ -7313,65 +7409,372 @@
       <c r="A199" s="1">
         <v>198</v>
       </c>
+      <c r="B199" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D199" s="1">
+        <v>-189.28</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F199" s="1">
+        <f>F198+D199</f>
+        <v>1500.1900000000003</v>
+      </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>199</v>
       </c>
+      <c r="B200" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D200" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F200" s="1">
+        <f>F199+D200</f>
+        <v>1485.1900000000003</v>
+      </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>200</v>
       </c>
+      <c r="B201" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D201" s="1">
+        <v>-28</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F201" s="1">
+        <f>F200+D201</f>
+        <v>1457.1900000000003</v>
+      </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>201</v>
       </c>
+      <c r="B202" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D202" s="1">
+        <v>-29.4</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F202" s="1">
+        <f>F201+D202</f>
+        <v>1427.7900000000002</v>
+      </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>202</v>
       </c>
+      <c r="B203" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D203" s="1">
+        <v>-32.5</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F203" s="1">
+        <f>F202+D203</f>
+        <v>1395.2900000000002</v>
+      </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>203</v>
       </c>
+      <c r="B204" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D204" s="1">
+        <v>-20.420000000000002</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F204" s="1">
+        <f>F203+D204</f>
+        <v>1374.8700000000001</v>
+      </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>204</v>
       </c>
+      <c r="B205" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D205" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F205" s="1">
+        <f>F204+D205</f>
+        <v>1372.8700000000001</v>
+      </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>205</v>
       </c>
+      <c r="B206" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D206" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F206" s="1">
+        <f>F205+D206</f>
+        <v>1370.8700000000001</v>
+      </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>206</v>
       </c>
+      <c r="B207" s="8">
+        <v>45628</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D207" s="4">
+        <f>SUM(D197:D206)</f>
+        <v>-434</v>
+      </c>
+      <c r="E207" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F207" s="4">
+        <f>F206</f>
+        <v>1370.8700000000001</v>
+      </c>
+      <c r="G207" s="4"/>
+      <c r="H207" s="4"/>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B208" s="8">
+        <v>45629</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D208" s="1">
+        <v>100</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F208" s="1">
+        <f>F207+D208</f>
+        <v>1470.8700000000001</v>
+      </c>
+      <c r="G208" s="1">
+        <v>-100</v>
+      </c>
+      <c r="H208" s="1">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B209" s="8">
+        <v>45629</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D209" s="1">
+        <v>-3</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F209" s="1">
+        <f>F208+D209</f>
+        <v>1467.8700000000001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B210" s="8">
+        <v>45629</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D210" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F210" s="1">
+        <f>F209+D210</f>
+        <v>1452.8700000000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>210</v>
+      </c>
+      <c r="B211" s="8">
+        <v>45629</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D211" s="1">
+        <v>-22.48</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F211" s="1">
+        <f>F210+D211</f>
+        <v>1430.39</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A212" s="1">
+        <v>211</v>
+      </c>
+      <c r="B212" s="8">
+        <v>45629</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D212" s="4">
+        <f>SUM(D209:D211)</f>
+        <v>-40.480000000000004</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F212" s="4">
+        <f>F211</f>
+        <v>1430.39</v>
+      </c>
+      <c r="G212" s="4"/>
+      <c r="H212" s="4"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A213" s="1">
+        <v>212</v>
+      </c>
+      <c r="B213" s="8">
+        <v>45630</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D213" s="1">
+        <v>-9.1</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F213" s="1">
+        <f>F212+D213</f>
+        <v>1421.2900000000002</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A214" s="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A215" s="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A216" s="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A217" s="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A218" s="1">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A219" s="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A220" s="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A221" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A222" s="1">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -7379,7 +7782,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="D58 D193" formulaRange="1"/>
-    <ignoredError sqref="F73 F167 F171 F177 F189 F193" formula="1"/>
+    <ignoredError sqref="F73 F167 F171 F177 F189 F193 F207 F212" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
data update 12.9 with previous commitment push failure re-push
</commit_message>
<xml_diff>
--- a/November.xlsx
+++ b/November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_project\py-db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E3EE2D-E4B6-4355-A284-95DFA3D726E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FED3A7-305F-46E7-9E61-4E983EF0C187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="25820" windowHeight="15620" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="337">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1329,6 +1329,50 @@
   </si>
   <si>
     <t>小食+上回买的小水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从学校到澡堂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吃吃M记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从澡堂旁的M回学校</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经典套餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迅雷会员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个月送航旅月卡</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3294,7 +3338,7 @@
   <dimension ref="A1:H245"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A213" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E232" sqref="E232"/>
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8383,43 +8427,142 @@
       <c r="A237" s="1">
         <v>236</v>
       </c>
+      <c r="B237" s="8">
+        <v>45634</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D237" s="1">
+        <v>-7.49</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F237" s="1">
+        <f>F236+D237</f>
+        <v>1318.1200000000001</v>
+      </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>237</v>
       </c>
+      <c r="B238" s="8">
+        <v>45634</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D238" s="1">
+        <v>-27.8</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F238" s="1">
+        <f>F237+D238</f>
+        <v>1290.3200000000002</v>
+      </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>238</v>
       </c>
+      <c r="B239" s="8">
+        <v>45634</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D239" s="1">
+        <v>-7.47</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F239" s="1">
+        <f>F238+D239</f>
+        <v>1282.8500000000001</v>
+      </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B240" s="8">
+        <v>45634</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D240" s="4">
+        <f>SUM(D236:D239)</f>
+        <v>-57.760000000000005</v>
+      </c>
+      <c r="E240" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F240" s="4">
+        <f>F239</f>
+        <v>1282.8500000000001</v>
+      </c>
+      <c r="G240" s="4"/>
+      <c r="H240" s="4"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B241" s="8">
+        <v>45635</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D241" s="1">
+        <v>-9.1</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F241" s="1">
+        <f>F240+D241</f>
+        <v>1273.7500000000002</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>241</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B242" s="8">
+        <v>45635</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D242" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F242" s="1">
+        <f>F241+D242</f>
+        <v>1243.7500000000002</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>244</v>
       </c>

</xml_diff>

<commit_message>
fix:figure data display error and data update 12.25 with a long gap for my contest to get a Master degree.
</commit_message>
<xml_diff>
--- a/November.xlsx
+++ b/November.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py_project\py-db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A855A4E8-CC6C-4D49-873B-B89A10B017B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D806E2-618A-4E90-B2CC-94EE6CDDCD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="25820" windowHeight="15620" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{B8BF14AF-E44B-4416-958B-4432C437B52F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="449">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1625,6 +1625,202 @@
   </si>
   <si>
     <t>回归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有吵翻了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这回是打印</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收获</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上间餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>起的晚，稍微多休息了一下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>库迪不如瑞幸啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红包熊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早上没起太早吃了个早午饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>走地铁过道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>md没注意可以不进去草了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前往酒店</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羊肉汤面（冬至前晚吃一个）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买瓶水喝喝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天是考试前一天，重点开销在行车和吃饭上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中午从考点回酒店吃饭（也算是得到哪哪人都多的教训了）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吃的黏糊麻辣烫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？我也不知道买了个啥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吃的小碗菜，那个b红烧鳕鱼真jb难吃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饮料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜜雪的冰淇淋和奶绿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天是开始的第一天，属于是大头在吃上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉妈妈打卤面，还不错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打印准考证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>踩考点那天记过来了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从酒店到仁风阁（朝鲜将军产业）吃饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这只是毛巾加一瓶水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从绿园到新天地附近</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注：还有一些信贷消费没入账</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>就目前看来消费也一般</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从电竞酒店到酒店收拾东西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一顿学校食堂了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分赃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饭钱和烧烤钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坤的分量回给我</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凑一凑给兔兔买新衣服（能忍住不买的都是神人）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个是专业课考试前买的咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1L的百岁山</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从学校到长春站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火车站的神奇定价（350ml）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subway</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神奇三明治，沟槽的定价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寄衣服</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>委托张兄寄出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>什么结息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>明天将记录所有信贷消费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机酒合一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电竞酒店</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3587,26 +3783,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5B7EDF-6532-4014-9E3B-D49D9FBA2851}">
-  <dimension ref="A1:H301"/>
+  <dimension ref="A1:H360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D288" sqref="D288"/>
+    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E299" sqref="E299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="55.9140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.08203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="55.875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="1"/>
+    <col min="10" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>103</v>
       </c>
@@ -3632,7 +3828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3656,7 +3852,7 @@
         <v>1846.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3678,7 +3874,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3700,7 +3896,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3722,7 +3918,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3744,7 +3940,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3762,7 +3958,7 @@
         <v>937.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3783,7 +3979,7 @@
         <v>935.80000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3804,7 +4000,7 @@
         <v>934.00000000000011</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3825,7 +4021,7 @@
         <v>925.50000000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3846,7 +4042,7 @@
         <v>922.70000000000016</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3867,7 +4063,7 @@
         <v>906.2600000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3888,7 +4084,7 @@
         <v>883.96000000000015</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3909,7 +4105,7 @@
         <v>863.96000000000015</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3927,7 +4123,7 @@
         <v>863.96000000000015</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3948,7 +4144,7 @@
         <v>839.06000000000017</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3969,7 +4165,7 @@
         <v>835.26000000000022</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3990,7 +4186,7 @@
         <v>830.26000000000022</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4011,7 +4207,7 @@
         <v>817.26000000000022</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4032,7 +4228,7 @@
         <v>752.38000000000022</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4053,7 +4249,7 @@
         <v>740.10000000000025</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4074,7 +4270,7 @@
         <v>734.10000000000025</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4095,7 +4291,7 @@
         <v>721.10000000000025</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4116,7 +4312,7 @@
         <v>709.10000000000025</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4137,7 +4333,7 @@
         <v>708.10000000000025</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4158,7 +4354,7 @@
         <v>678.10000000000025</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4176,7 +4372,7 @@
         <v>678.1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4197,7 +4393,7 @@
         <v>648.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4218,7 +4414,7 @@
         <v>644.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4239,7 +4435,7 @@
         <v>639.1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4260,7 +4456,7 @@
         <v>629.79000000000008</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4281,7 +4477,7 @@
         <v>628.45000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4302,7 +4498,7 @@
         <v>618.45000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4323,7 +4519,7 @@
         <v>610.95000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4344,7 +4540,7 @@
         <v>575.95000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4365,7 +4561,7 @@
         <v>562.95000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4386,7 +4582,7 @@
         <v>560.45000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4404,7 +4600,7 @@
         <v>560.45000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4425,7 +4621,7 @@
         <v>553.05000000000007</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4446,7 +4642,7 @@
         <v>540.05000000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4467,7 +4663,7 @@
         <v>538.05000000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4495,7 +4691,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4516,7 +4712,7 @@
         <v>577.65000000000009</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4537,7 +4733,7 @@
         <v>571.65000000000009</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4555,7 +4751,7 @@
         <v>571.65000000000009</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4576,7 +4772,7 @@
         <v>563.95000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4597,7 +4793,7 @@
         <v>553.95000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4618,7 +4814,7 @@
         <v>545.95000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4639,7 +4835,7 @@
         <v>535.95000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4657,7 +4853,7 @@
         <v>535.95000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4678,7 +4874,7 @@
         <v>529.95000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -4699,7 +4895,7 @@
         <v>521.45000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4720,7 +4916,7 @@
         <v>475.91</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4741,7 +4937,7 @@
         <v>472.31</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4762,7 +4958,7 @@
         <v>462.31</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4789,7 +4985,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4810,7 +5006,7 @@
         <v>542.30999999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4828,7 +5024,7 @@
         <v>542.30999999999995</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4849,7 +5045,7 @@
         <v>496.30999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4870,7 +5066,7 @@
         <v>484.30999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4888,7 +5084,7 @@
         <v>484.30999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4909,7 +5105,7 @@
         <v>481.60999999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4936,7 +5132,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4957,7 +5153,7 @@
         <v>579.80999999999995</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4978,7 +5174,7 @@
         <v>544.02</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -5005,7 +5201,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -5023,7 +5219,7 @@
         <v>944.02</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -5044,7 +5240,7 @@
         <v>942.22</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -5065,7 +5261,7 @@
         <v>927.22</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -5086,7 +5282,7 @@
         <v>922.22</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -5107,7 +5303,7 @@
         <v>917.22</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -5128,7 +5324,7 @@
         <v>897.22</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -5149,7 +5345,7 @@
         <v>897.22</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -5170,7 +5366,7 @@
         <v>875.22</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -5191,7 +5387,7 @@
         <v>873.22</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -5212,7 +5408,7 @@
         <v>861.22</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -5233,7 +5429,7 @@
         <v>840.22</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -5254,7 +5450,7 @@
         <v>840.22</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -5275,7 +5471,7 @@
         <v>820.22</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -5296,7 +5492,7 @@
         <v>818.22</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5317,7 +5513,7 @@
         <v>809.72</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5338,7 +5534,7 @@
         <v>809.72</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5359,7 +5555,7 @@
         <v>802.32</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5380,7 +5576,7 @@
         <v>796.5200000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5401,7 +5597,7 @@
         <v>785.5200000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5422,7 +5618,7 @@
         <v>785.5200000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5443,7 +5639,7 @@
         <v>782.5200000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5464,7 +5660,7 @@
         <v>760.5200000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5487,7 +5683,7 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5508,7 +5704,7 @@
         <v>730.5200000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5529,7 +5725,7 @@
         <v>723.12000000000012</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5552,7 +5748,7 @@
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5573,7 +5769,7 @@
         <v>693.32000000000016</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5594,7 +5790,7 @@
         <v>693.32000000000016</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5617,7 +5813,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5638,7 +5834,7 @@
         <v>658.32000000000016</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5659,7 +5855,7 @@
         <v>655.82000000000016</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5680,7 +5876,7 @@
         <v>630.82000000000016</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5703,7 +5899,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -5724,7 +5920,7 @@
         <v>627.62000000000012</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5745,7 +5941,7 @@
         <v>621.62000000000012</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -5766,7 +5962,7 @@
         <v>619.82000000000016</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5787,7 +5983,7 @@
         <v>596.72000000000014</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5810,7 +6006,7 @@
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5831,7 +6027,7 @@
         <v>596.42000000000019</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -5852,7 +6048,7 @@
         <v>580.42000000000019</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5873,7 +6069,7 @@
         <v>560.62000000000023</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -5896,7 +6092,7 @@
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5917,7 +6113,7 @@
         <v>559.62000000000023</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -5938,7 +6134,7 @@
         <v>537.62000000000023</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -5959,7 +6155,7 @@
         <v>535.62000000000023</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -5980,7 +6176,7 @@
         <v>502.05000000000024</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6001,7 +6197,7 @@
         <v>492.05000000000024</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6022,7 +6218,7 @@
         <v>490.25000000000023</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6043,7 +6239,7 @@
         <v>473.85000000000025</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6064,7 +6260,7 @@
         <v>468.85000000000025</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -6087,7 +6283,7 @@
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -6108,7 +6304,7 @@
         <v>461.45000000000027</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -6129,7 +6325,7 @@
         <v>450.45000000000027</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -6150,7 +6346,7 @@
         <v>445.45000000000027</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -6173,7 +6369,7 @@
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -6194,7 +6390,7 @@
         <v>431.45000000000027</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -6215,7 +6411,7 @@
         <v>413.45000000000027</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -6238,7 +6434,7 @@
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -6259,7 +6455,7 @@
         <v>407.25000000000028</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -6280,7 +6476,7 @@
         <v>387.5500000000003</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -6303,7 +6499,7 @@
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -6324,7 +6520,7 @@
         <v>380.0500000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -6345,7 +6541,7 @@
         <v>365.0500000000003</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -6366,7 +6562,7 @@
         <v>365.0500000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -6387,7 +6583,7 @@
         <v>357.25000000000028</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -6408,7 +6604,7 @@
         <v>351.25000000000028</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -6429,7 +6625,7 @@
         <v>349.25000000000028</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -6450,7 +6646,7 @@
         <v>347.25000000000028</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -6471,7 +6667,7 @@
         <v>325.25000000000028</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -6498,7 +6694,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -6519,7 +6715,7 @@
         <v>325.25000000000028</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -6540,7 +6736,7 @@
         <v>319.25000000000028</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -6561,7 +6757,7 @@
         <v>303.25000000000028</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -6584,7 +6780,7 @@
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -6605,7 +6801,7 @@
         <v>290.25000000000028</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -6626,7 +6822,7 @@
         <v>284.25000000000028</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -6647,7 +6843,7 @@
         <v>262.85000000000031</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -6670,7 +6866,7 @@
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -6691,7 +6887,7 @@
         <v>249.85000000000031</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -6712,7 +6908,7 @@
         <v>246.35000000000031</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -6733,7 +6929,7 @@
         <v>225.46000000000032</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -6754,7 +6950,7 @@
         <v>625.46000000000026</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -6777,7 +6973,7 @@
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -6798,7 +6994,7 @@
         <v>620.06000000000029</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -6819,7 +7015,7 @@
         <v>612.06000000000029</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -6840,7 +7036,7 @@
         <v>608.76000000000033</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -6861,7 +7057,7 @@
         <v>448.63000000000034</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -6882,7 +7078,7 @@
         <v>433.63000000000034</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -6909,7 +7105,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -6932,7 +7128,7 @@
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -6953,7 +7149,7 @@
         <v>433.63000000000034</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -6974,7 +7170,7 @@
         <v>421.63000000000034</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -6995,7 +7191,7 @@
         <v>416.63000000000034</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -7016,7 +7212,7 @@
         <v>394.85000000000036</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -7039,7 +7235,7 @@
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -7060,7 +7256,7 @@
         <v>393.85000000000036</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -7081,7 +7277,7 @@
         <v>386.35000000000036</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -7102,7 +7298,7 @@
         <v>381.00000000000034</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -7123,7 +7319,7 @@
         <v>362.00000000000034</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -7144,7 +7340,7 @@
         <v>360.00000000000034</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -7168,7 +7364,7 @@
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -7189,7 +7385,7 @@
         <v>345.00000000000034</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -7210,7 +7406,7 @@
         <v>322.52000000000032</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -7231,7 +7427,7 @@
         <v>332.52000000000032</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -7255,7 +7451,7 @@
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -7276,7 +7472,7 @@
         <v>323.4200000000003</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -7297,7 +7493,7 @@
         <v>313.52000000000032</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -7318,7 +7514,7 @@
         <v>298.52000000000032</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -7339,7 +7535,7 @@
         <v>276.52000000000032</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -7360,7 +7556,7 @@
         <v>258.52000000000032</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -7384,7 +7580,7 @@
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -7405,7 +7601,7 @@
         <v>257.4200000000003</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -7426,7 +7622,7 @@
         <v>78.4200000000003</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -7447,7 +7643,7 @@
         <v>76.620000000000303</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -7468,7 +7664,7 @@
         <v>62.630000000000301</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -7489,7 +7685,7 @@
         <v>58.630000000000301</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -7510,7 +7706,7 @@
         <v>54.630000000000301</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -7531,7 +7727,7 @@
         <v>33.340000000000302</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -7552,7 +7748,7 @@
         <v>34.440000000000303</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -7573,7 +7769,7 @@
         <v>124.44000000000031</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -7594,7 +7790,7 @@
         <v>89.510000000000304</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -7615,7 +7811,7 @@
         <v>17.650000000000304</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -7643,7 +7839,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -7664,7 +7860,7 @@
         <v>1017.6500000000003</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -7685,7 +7881,7 @@
         <v>995.1700000000003</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -7706,7 +7902,7 @@
         <v>964.87000000000035</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -7730,7 +7926,7 @@
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -7751,7 +7947,7 @@
         <v>1184.8700000000003</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -7772,7 +7968,7 @@
         <v>1584.8700000000003</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -7799,7 +7995,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -7820,7 +8016,7 @@
         <v>1696.8700000000003</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -7841,7 +8037,7 @@
         <v>1689.4700000000003</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -7862,7 +8058,7 @@
         <v>1500.1900000000003</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -7883,7 +8079,7 @@
         <v>1485.1900000000003</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -7904,7 +8100,7 @@
         <v>1457.1900000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -7925,7 +8121,7 @@
         <v>1427.7900000000002</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -7946,7 +8142,7 @@
         <v>1395.2900000000002</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -7967,7 +8163,7 @@
         <v>1374.8700000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -7988,7 +8184,7 @@
         <v>1372.8700000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -8009,7 +8205,7 @@
         <v>1370.8700000000001</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -8033,7 +8229,7 @@
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -8060,7 +8256,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -8081,7 +8277,7 @@
         <v>1467.8700000000001</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -8102,7 +8298,7 @@
         <v>1452.8700000000001</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -8123,7 +8319,7 @@
         <v>1430.39</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -8147,7 +8343,7 @@
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -8168,7 +8364,7 @@
         <v>1421.2900000000002</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -8189,7 +8385,7 @@
         <v>1701.2900000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -8216,7 +8412,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -8237,7 +8433,7 @@
         <v>1408.8100000000002</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -8258,7 +8454,7 @@
         <v>1398.91</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -8282,7 +8478,7 @@
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -8309,7 +8505,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -8330,7 +8526,7 @@
         <v>1442.93</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -8351,7 +8547,7 @@
         <v>1425.39</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -8372,7 +8568,7 @@
         <v>1402.71</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -8393,7 +8589,7 @@
         <v>1391.91</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -8414,7 +8610,7 @@
         <v>1391.91</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -8435,7 +8631,7 @@
         <v>1411.01</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -8459,7 +8655,7 @@
       <c r="G226" s="4"/>
       <c r="H226" s="4"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -8480,7 +8676,7 @@
         <v>1401.21</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -8501,7 +8697,7 @@
         <v>1397.6100000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -8522,7 +8718,7 @@
         <v>1395.6100000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -8543,7 +8739,7 @@
         <v>1385.6100000000001</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -8564,7 +8760,7 @@
         <v>1370.6100000000001</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -8588,7 +8784,7 @@
       <c r="G232" s="4"/>
       <c r="H232" s="4"/>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -8609,7 +8805,7 @@
         <v>1350.6100000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -8630,7 +8826,7 @@
         <v>1340.6100000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -8654,7 +8850,7 @@
       <c r="G235" s="4"/>
       <c r="H235" s="4"/>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -8675,7 +8871,7 @@
         <v>1325.6100000000001</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -8696,7 +8892,7 @@
         <v>1318.1200000000001</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -8717,7 +8913,7 @@
         <v>1290.3200000000002</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -8738,7 +8934,7 @@
         <v>1282.8500000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -8762,7 +8958,7 @@
       <c r="G240" s="4"/>
       <c r="H240" s="4"/>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -8783,7 +8979,7 @@
         <v>1273.7500000000002</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -8804,7 +9000,7 @@
         <v>1243.7500000000002</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -8825,7 +9021,7 @@
         <v>1228.7500000000002</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -8849,7 +9045,7 @@
       <c r="G244" s="4"/>
       <c r="H244" s="4"/>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -8876,7 +9072,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -8897,7 +9093,7 @@
         <v>1613.7500000000002</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -8918,7 +9114,7 @@
         <v>1591.9000000000003</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -8939,7 +9135,7 @@
         <v>1590.1000000000004</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -8960,7 +9156,7 @@
         <v>1586.9700000000003</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -8981,7 +9177,7 @@
         <v>1569.0700000000002</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -9002,7 +9198,7 @@
         <v>1549.5800000000002</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -9023,7 +9219,7 @@
         <v>1540.9800000000002</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -9047,7 +9243,7 @@
       <c r="G253" s="4"/>
       <c r="H253" s="4"/>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -9068,7 +9264,7 @@
         <v>1539.1800000000003</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -9089,7 +9285,7 @@
         <v>1535.3800000000003</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -9110,7 +9306,7 @@
         <v>1533.2800000000004</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -9131,7 +9327,7 @@
         <v>1532.4800000000005</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -9152,7 +9348,7 @@
         <v>1525.9800000000005</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -9176,7 +9372,7 @@
       <c r="G259" s="4"/>
       <c r="H259" s="4"/>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -9197,7 +9393,7 @@
         <v>1516.5800000000004</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -9218,7 +9414,7 @@
         <v>1477.0800000000004</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -9239,7 +9435,7 @@
         <v>1399.0800000000004</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -9260,7 +9456,7 @@
         <v>1306.2000000000003</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -9287,7 +9483,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>264</v>
       </c>
@@ -9311,7 +9507,7 @@
       <c r="G265" s="4"/>
       <c r="H265" s="4"/>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
@@ -9338,7 +9534,7 @@
         <v>4170</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
@@ -9365,7 +9561,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
@@ -9386,7 +9582,7 @@
         <v>1201.9100000000003</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
@@ -9407,7 +9603,7 @@
         <v>1189.9100000000003</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
@@ -9428,7 +9624,7 @@
         <v>1110.5100000000002</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>270</v>
       </c>
@@ -9449,7 +9645,7 @@
         <v>1108.0100000000002</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>271</v>
       </c>
@@ -9470,7 +9666,7 @@
         <v>1099.0100000000002</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>272</v>
       </c>
@@ -9494,7 +9690,7 @@
       <c r="G273" s="4"/>
       <c r="H273" s="4"/>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -9515,7 +9711,7 @@
         <v>1095.2100000000003</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -9536,7 +9732,7 @@
         <v>1080.2100000000003</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
@@ -9557,7 +9753,7 @@
         <v>1071.2000000000003</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
@@ -9578,7 +9774,7 @@
         <v>1050.3300000000004</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
@@ -9599,7 +9795,7 @@
         <v>1021.3300000000004</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>278</v>
       </c>
@@ -9620,7 +9816,7 @@
         <v>1018.3300000000004</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
@@ -9641,7 +9837,7 @@
         <v>989.4300000000004</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>280</v>
       </c>
@@ -9662,7 +9858,7 @@
         <v>984.8100000000004</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>281</v>
       </c>
@@ -9686,7 +9882,7 @@
       <c r="G282" s="4"/>
       <c r="H282" s="4"/>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>282</v>
       </c>
@@ -9707,7 +9903,7 @@
         <v>975.8100000000004</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>283</v>
       </c>
@@ -9728,7 +9924,7 @@
         <v>963.8100000000004</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
@@ -9749,7 +9945,7 @@
         <v>951.8100000000004</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>285</v>
       </c>
@@ -9773,7 +9969,7 @@
       <c r="G286" s="4"/>
       <c r="H286" s="4"/>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>286</v>
       </c>
@@ -9794,7 +9990,7 @@
         <v>942.41000000000042</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>287</v>
       </c>
@@ -9815,7 +10011,7 @@
         <v>938.91000000000042</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>288</v>
       </c>
@@ -9836,7 +10032,7 @@
         <v>835.91000000000042</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -9857,7 +10053,7 @@
         <v>834.11000000000047</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>290</v>
       </c>
@@ -9878,7 +10074,7 @@
         <v>809.76000000000045</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -9899,7 +10095,7 @@
         <v>794.26000000000045</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>292</v>
       </c>
@@ -9920,7 +10116,7 @@
         <v>772.16000000000042</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>293</v>
       </c>
@@ -9944,12 +10140,12 @@
       <c r="G294" s="4"/>
       <c r="H294" s="4"/>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>294</v>
       </c>
       <c r="B295" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>20</v>
@@ -9965,12 +10161,12 @@
         <v>757.16000000000042</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>295</v>
       </c>
       <c r="B296" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>17</v>
@@ -9986,12 +10182,12 @@
         <v>755.36000000000047</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>296</v>
       </c>
       <c r="B297" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>12</v>
@@ -10007,12 +10203,12 @@
         <v>743.36000000000047</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>297</v>
       </c>
       <c r="B298" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>398</v>
@@ -10028,12 +10224,12 @@
         <v>733.46000000000049</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
       <c r="B299" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>65</v>
@@ -10049,12 +10245,12 @@
         <v>731.46000000000049</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>299</v>
       </c>
       <c r="B300" s="8">
-        <v>45613</v>
+        <v>45643</v>
       </c>
       <c r="C300" s="4" t="s">
         <v>15</v>
@@ -10073,12 +10269,1243 @@
       <c r="G300" s="4"/>
       <c r="H300" s="4"/>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>300</v>
       </c>
       <c r="B301" s="8">
         <v>45644</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D301" s="1">
+        <v>-7.8</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F301" s="1">
+        <f t="shared" ref="F301:F306" si="15">F300+D301</f>
+        <v>723.66000000000054</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>301</v>
+      </c>
+      <c r="B302" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D302" s="1">
+        <v>-31.12</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F302" s="1">
+        <f t="shared" si="15"/>
+        <v>692.54000000000053</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>302</v>
+      </c>
+      <c r="B303" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D303" s="1">
+        <v>-3.5</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F303" s="1">
+        <f t="shared" si="15"/>
+        <v>689.04000000000053</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>303</v>
+      </c>
+      <c r="B304" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D304" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F304" s="1">
+        <f t="shared" si="15"/>
+        <v>674.04000000000053</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A305" s="1">
+        <v>304</v>
+      </c>
+      <c r="B305" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D305" s="1">
+        <v>4.13</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F305" s="1">
+        <f t="shared" si="15"/>
+        <v>678.17000000000053</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>305</v>
+      </c>
+      <c r="B306" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D306" s="1">
+        <v>-9</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F306" s="1">
+        <f t="shared" si="15"/>
+        <v>669.17000000000053</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>306</v>
+      </c>
+      <c r="B307" s="8">
+        <v>45644</v>
+      </c>
+      <c r="C307" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D307" s="4">
+        <f>SUM(D301:D306)</f>
+        <v>-62.29</v>
+      </c>
+      <c r="E307" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F307" s="4">
+        <f>F306</f>
+        <v>669.17000000000053</v>
+      </c>
+      <c r="G307" s="4"/>
+      <c r="H307" s="4"/>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>307</v>
+      </c>
+      <c r="B308" s="8">
+        <v>45645</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D308" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="F308" s="1">
+        <f>F307+D308</f>
+        <v>654.17000000000053</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>308</v>
+      </c>
+      <c r="B309" s="8">
+        <v>45645</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D309" s="1">
+        <v>-21.98</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F309" s="1">
+        <f>F308+D309</f>
+        <v>632.19000000000051</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>309</v>
+      </c>
+      <c r="B310" s="8">
+        <v>45645</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D310" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F310" s="1">
+        <f>F309+D310</f>
+        <v>617.19000000000051</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>310</v>
+      </c>
+      <c r="B311" s="8">
+        <v>45645</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D311" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F311" s="1">
+        <f>F310+D311</f>
+        <v>617.36000000000047</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>311</v>
+      </c>
+      <c r="B312" s="8">
+        <v>45645</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D312" s="4">
+        <f>SUM(D308:D311)</f>
+        <v>-51.81</v>
+      </c>
+      <c r="E312" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F312" s="4">
+        <f>F311</f>
+        <v>617.36000000000047</v>
+      </c>
+      <c r="G312" s="4"/>
+      <c r="H312" s="4"/>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A313" s="1">
+        <v>312</v>
+      </c>
+      <c r="B313" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D313" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F313" s="1">
+        <f t="shared" ref="F313:F319" si="16">F312+D313</f>
+        <v>602.36000000000047</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A314" s="1">
+        <v>313</v>
+      </c>
+      <c r="B314" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D314" s="1">
+        <v>-2</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F314" s="1">
+        <f t="shared" si="16"/>
+        <v>600.36000000000047</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A315" s="1">
+        <v>314</v>
+      </c>
+      <c r="B315" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D315" s="1">
+        <v>-31.96</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F315" s="1">
+        <f t="shared" si="16"/>
+        <v>568.40000000000043</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A316" s="1">
+        <v>315</v>
+      </c>
+      <c r="B316" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D316" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E316" s="1">
+        <v>1</v>
+      </c>
+      <c r="F316" s="1">
+        <f t="shared" si="16"/>
+        <v>563.40000000000043</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A317" s="1">
+        <v>316</v>
+      </c>
+      <c r="B317" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D317" s="1">
+        <v>-15.7</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F317" s="1">
+        <f t="shared" si="16"/>
+        <v>547.70000000000039</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A318" s="1">
+        <v>317</v>
+      </c>
+      <c r="B318" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D318" s="1">
+        <v>-25</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F318" s="1">
+        <f t="shared" si="16"/>
+        <v>522.70000000000039</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A319" s="1">
+        <v>318</v>
+      </c>
+      <c r="B319" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D319" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F319" s="1">
+        <f t="shared" si="16"/>
+        <v>521.20000000000039</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A320" s="1">
+        <v>319</v>
+      </c>
+      <c r="B320" s="8">
+        <v>45646</v>
+      </c>
+      <c r="C320" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D320" s="4">
+        <f>SUM(D313:D319)</f>
+        <v>-96.16</v>
+      </c>
+      <c r="E320" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="F320" s="4">
+        <f>F319</f>
+        <v>521.20000000000039</v>
+      </c>
+      <c r="G320" s="4"/>
+      <c r="H320" s="4"/>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A321" s="1">
+        <v>320</v>
+      </c>
+      <c r="B321" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D321" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E321" s="1">
+        <v>2</v>
+      </c>
+      <c r="F321" s="1">
+        <f t="shared" ref="F321:F327" si="17">F320+D321</f>
+        <v>516.20000000000039</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A322" s="1">
+        <v>321</v>
+      </c>
+      <c r="B322" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D322" s="1">
+        <v>-7.7</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F322" s="1">
+        <f t="shared" si="17"/>
+        <v>508.5000000000004</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A323" s="1">
+        <v>322</v>
+      </c>
+      <c r="B323" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D323" s="1">
+        <v>-24.21</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="F323" s="1">
+        <f t="shared" si="17"/>
+        <v>484.29000000000042</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A324" s="1">
+        <v>323</v>
+      </c>
+      <c r="B324" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D324" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F324" s="1">
+        <f t="shared" si="17"/>
+        <v>479.29000000000042</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A325" s="1">
+        <v>324</v>
+      </c>
+      <c r="B325" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D325" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E325" s="1">
+        <v>3</v>
+      </c>
+      <c r="F325" s="1">
+        <f t="shared" si="17"/>
+        <v>474.29000000000042</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A326" s="1">
+        <v>325</v>
+      </c>
+      <c r="B326" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D326" s="1">
+        <v>-24</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F326" s="1">
+        <f t="shared" si="17"/>
+        <v>450.29000000000042</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A327" s="1">
+        <v>326</v>
+      </c>
+      <c r="B327" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D327" s="1">
+        <v>-8</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F327" s="1">
+        <f t="shared" si="17"/>
+        <v>442.29000000000042</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A328" s="1">
+        <v>327</v>
+      </c>
+      <c r="B328" s="8">
+        <v>45647</v>
+      </c>
+      <c r="C328" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D328" s="4">
+        <f>SUM(D321:D327)</f>
+        <v>-78.91</v>
+      </c>
+      <c r="E328" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F328" s="4">
+        <f>F327</f>
+        <v>442.29000000000042</v>
+      </c>
+      <c r="G328" s="4"/>
+      <c r="H328" s="4"/>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A329" s="1">
+        <v>328</v>
+      </c>
+      <c r="B329" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D329" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E329" s="1">
+        <v>4</v>
+      </c>
+      <c r="F329" s="1">
+        <f t="shared" ref="F329:F336" si="18">F328+D329</f>
+        <v>437.29000000000042</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A330" s="1">
+        <v>329</v>
+      </c>
+      <c r="B330" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D330" s="1">
+        <v>-13</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F330" s="1">
+        <f t="shared" si="18"/>
+        <v>424.29000000000042</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>330</v>
+      </c>
+      <c r="B331" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D331" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="F331" s="1">
+        <f t="shared" si="18"/>
+        <v>423.79000000000042</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>331</v>
+      </c>
+      <c r="B332" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D332" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E332" s="1">
+        <v>5</v>
+      </c>
+      <c r="F332" s="1">
+        <f t="shared" si="18"/>
+        <v>418.79000000000042</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>332</v>
+      </c>
+      <c r="B333" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D333" s="1">
+        <v>-20.95</v>
+      </c>
+      <c r="E333" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F333" s="1">
+        <f t="shared" si="18"/>
+        <v>397.84000000000043</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>333</v>
+      </c>
+      <c r="B334" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D334" s="1">
+        <v>-13</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F334" s="1">
+        <f t="shared" si="18"/>
+        <v>384.84000000000043</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>334</v>
+      </c>
+      <c r="B335" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D335" s="1">
+        <v>-7.3</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F335" s="1">
+        <f t="shared" si="18"/>
+        <v>377.54000000000042</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A336" s="1">
+        <v>335</v>
+      </c>
+      <c r="B336" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D336" s="1">
+        <v>0</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F336" s="1">
+        <f t="shared" si="18"/>
+        <v>377.54000000000042</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>336</v>
+      </c>
+      <c r="B337" s="8">
+        <v>45648</v>
+      </c>
+      <c r="C337" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D337" s="4">
+        <f>SUM(D329:D336)</f>
+        <v>-64.75</v>
+      </c>
+      <c r="E337" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F337" s="4">
+        <f>F336</f>
+        <v>377.54000000000042</v>
+      </c>
+      <c r="G337" s="4"/>
+      <c r="H337" s="4"/>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A338" s="1">
+        <v>337</v>
+      </c>
+      <c r="B338" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D338" s="1">
+        <v>-9.35</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F338" s="1">
+        <f t="shared" ref="F338:F345" si="19">F337+D338</f>
+        <v>368.1900000000004</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A339" s="1">
+        <v>338</v>
+      </c>
+      <c r="B339" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D339" s="1">
+        <v>-15</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F339" s="1">
+        <f t="shared" si="19"/>
+        <v>353.1900000000004</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A340" s="1">
+        <v>339</v>
+      </c>
+      <c r="B340" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D340" s="1">
+        <v>-23.57</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F340" s="1">
+        <f t="shared" si="19"/>
+        <v>329.6200000000004</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A341" s="1">
+        <v>340</v>
+      </c>
+      <c r="B341" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D341" s="1">
+        <v>-97</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F341" s="1">
+        <f t="shared" si="19"/>
+        <v>232.6200000000004</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A342" s="1">
+        <v>341</v>
+      </c>
+      <c r="B342" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D342" s="1">
+        <v>66</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F342" s="1">
+        <f t="shared" si="19"/>
+        <v>298.6200000000004</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A343" s="1">
+        <v>342</v>
+      </c>
+      <c r="B343" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D343" s="1">
+        <v>-6</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F343" s="1">
+        <f t="shared" si="19"/>
+        <v>292.6200000000004</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A344" s="1">
+        <v>343</v>
+      </c>
+      <c r="B344" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D344" s="1">
+        <v>-24.96</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F344" s="1">
+        <f t="shared" si="19"/>
+        <v>267.66000000000042</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A345" s="1">
+        <v>344</v>
+      </c>
+      <c r="B345" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D345" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F345" s="1">
+        <f t="shared" si="19"/>
+        <v>237.66000000000042</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A346" s="1">
+        <v>345</v>
+      </c>
+      <c r="B346" s="8">
+        <v>45649</v>
+      </c>
+      <c r="C346" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D346" s="4">
+        <f>SUM(D338:D345)</f>
+        <v>-139.88000000000002</v>
+      </c>
+      <c r="E346" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F346" s="4">
+        <f>F345</f>
+        <v>237.66000000000042</v>
+      </c>
+      <c r="G346" s="4"/>
+      <c r="H346" s="4"/>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A347" s="1">
+        <v>346</v>
+      </c>
+      <c r="B347" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D347" s="1">
+        <v>-13.36</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F347" s="1">
+        <f t="shared" ref="F347:F353" si="20">F346+D347</f>
+        <v>224.30000000000041</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A348" s="1">
+        <v>347</v>
+      </c>
+      <c r="B348" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D348" s="1">
+        <v>-3.9</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F348" s="1">
+        <f t="shared" si="20"/>
+        <v>220.4000000000004</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A349" s="1">
+        <v>348</v>
+      </c>
+      <c r="B349" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D349" s="1">
+        <v>-22.9</v>
+      </c>
+      <c r="E349" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F349" s="1">
+        <f t="shared" si="20"/>
+        <v>197.5000000000004</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A350" s="1">
+        <v>349</v>
+      </c>
+      <c r="B350" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D350" s="1">
+        <v>-2.5</v>
+      </c>
+      <c r="E350" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F350" s="1">
+        <f t="shared" si="20"/>
+        <v>195.0000000000004</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A351" s="1">
+        <v>350</v>
+      </c>
+      <c r="B351" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D351" s="1">
+        <v>-49</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F351" s="1">
+        <f t="shared" si="20"/>
+        <v>146.0000000000004</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
+        <v>351</v>
+      </c>
+      <c r="B352" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D352" s="1">
+        <v>-20</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F352" s="1">
+        <f t="shared" si="20"/>
+        <v>126.0000000000004</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A353" s="1">
+        <v>352</v>
+      </c>
+      <c r="B353" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D353" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F353" s="1">
+        <f t="shared" si="20"/>
+        <v>126.0400000000004</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A354" s="1">
+        <v>353</v>
+      </c>
+      <c r="B354" s="8">
+        <v>45650</v>
+      </c>
+      <c r="C354" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D354" s="4">
+        <f>SUM(D347:D353)</f>
+        <v>-111.61999999999999</v>
+      </c>
+      <c r="E354" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="F354" s="4">
+        <f>F353</f>
+        <v>126.0400000000004</v>
+      </c>
+      <c r="G354" s="4"/>
+      <c r="H354" s="4"/>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A355" s="1">
+        <v>354</v>
+      </c>
+      <c r="B355" s="8">
+        <v>45651</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D355" s="1">
+        <v>2600</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F355" s="1">
+        <f>F354+D355</f>
+        <v>2726.0400000000004</v>
+      </c>
+      <c r="G355" s="1">
+        <v>-2600</v>
+      </c>
+      <c r="H355" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A356" s="1">
+        <v>355</v>
+      </c>
+      <c r="B356" s="8">
+        <v>45651</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D356" s="1">
+        <v>-1965.76</v>
+      </c>
+      <c r="E356" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F356" s="1">
+        <f>F355+D356</f>
+        <v>760.28000000000043</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A357" s="1">
+        <v>356</v>
+      </c>
+      <c r="B357" s="8">
+        <v>45651</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D357" s="1">
+        <v>-205.85</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F357" s="1">
+        <f>F356+D357</f>
+        <v>554.4300000000004</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A358" s="1">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A359" s="1">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A360" s="1">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -10099,16 +11526,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.9140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.58203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="40.75" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="1"/>
+    <col min="5" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -10116,7 +11543,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -10130,7 +11557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
@@ -10141,7 +11568,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -10152,7 +11579,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -10163,7 +11590,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6" s="1">
         <f>SUM(C3:C5)</f>
         <v>24.4</v>

</xml_diff>